<commit_message>
UPDATED:  public categs excel & json
</commit_message>
<xml_diff>
--- a/data/common/excel/public_categories_odoo.xlsx
+++ b/data/common/excel/public_categories_odoo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OPT Design\PycharmProjects\optima-scrapper\data\common\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD9F71F-3E1A-4F22-A542-C9BD7795C1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8860971-77A5-46D9-AA16-E00B53CEDF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32325" yWindow="1560" windowWidth="18930" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="87">
   <si>
     <t>ACCESORIOS PARA LINEALES MAGNETICOS</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>BOMBILLAS LED SOLAR CON SENSOR</t>
+  </si>
+  <si>
+    <t>NEONES LED</t>
   </si>
 </sst>
 </file>
@@ -631,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,1068 +662,1079 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>10000</v>
-      </c>
-      <c r="B2" s="2">
-        <v>12</v>
-      </c>
+        <v>10105</v>
+      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>10005</v>
-      </c>
-      <c r="B3" s="2">
-        <v>20</v>
-      </c>
+        <v>10110</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>10010</v>
-      </c>
-      <c r="B4" s="2">
-        <v>6</v>
-      </c>
+        <v>10115</v>
+      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>10015</v>
-      </c>
-      <c r="B5" s="2">
-        <v>11</v>
-      </c>
+        <v>10120</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>10020</v>
-      </c>
-      <c r="B6" s="2">
-        <v>9</v>
-      </c>
+        <v>10125</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>10025</v>
-      </c>
-      <c r="B7" s="2">
-        <v>17</v>
-      </c>
+        <v>10130</v>
+      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>63</v>
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>10030</v>
-      </c>
-      <c r="B8" s="2">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>54</v>
+        <v>10135</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>10035</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
+        <v>10140</v>
+      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>58</v>
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>10040</v>
-      </c>
-      <c r="B10" s="2">
-        <v>13</v>
-      </c>
+        <v>10145</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>84</v>
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>10045</v>
-      </c>
-      <c r="B11" s="2">
-        <v>19</v>
-      </c>
+        <v>10150</v>
+      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>10050</v>
-      </c>
-      <c r="B12" s="2">
-        <v>4</v>
-      </c>
+        <v>10155</v>
+      </c>
+      <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>81</v>
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>10055</v>
-      </c>
-      <c r="B13" s="2">
-        <v>18</v>
-      </c>
+        <v>10160</v>
+      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>10060</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
+        <v>10165</v>
+      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>10065</v>
-      </c>
-      <c r="B15" s="2">
-        <v>15</v>
-      </c>
+        <v>10170</v>
+      </c>
+      <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>62</v>
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>10070</v>
-      </c>
-      <c r="B16" s="2">
-        <v>7</v>
-      </c>
+        <v>10175</v>
+      </c>
+      <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>10075</v>
-      </c>
-      <c r="B17" s="2">
-        <v>10</v>
-      </c>
+        <v>10180</v>
+      </c>
+      <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>10080</v>
-      </c>
-      <c r="B18" s="2">
-        <v>14</v>
-      </c>
+        <v>10185</v>
+      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>10085</v>
-      </c>
-      <c r="B19" s="2">
-        <v>2</v>
-      </c>
+        <v>10190</v>
+      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>10090</v>
-      </c>
-      <c r="B20" s="2">
-        <v>8</v>
-      </c>
+        <v>10195</v>
+      </c>
+      <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>83</v>
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>10095</v>
-      </c>
-      <c r="B21" s="2">
-        <v>5</v>
-      </c>
+        <v>10200</v>
+      </c>
+      <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>10100</v>
+        <v>10205</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>10105</v>
+        <v>10210</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>10110</v>
+        <v>10215</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>10115</v>
+        <v>10220</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>10120</v>
+        <v>10225</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>10125</v>
+        <v>10230</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>10130</v>
+        <v>10235</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>10135</v>
+        <v>10240</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>10140</v>
+        <v>10245</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>10145</v>
+        <v>10250</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>10150</v>
+        <v>10255</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>10155</v>
+        <v>10260</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>10160</v>
+        <v>10265</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>10165</v>
+        <v>10270</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>10170</v>
+        <v>10275</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>10175</v>
+        <v>10280</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>10180</v>
+        <v>10285</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>10185</v>
+        <v>10290</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>10190</v>
+        <v>10295</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>10195</v>
+        <v>10300</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>10200</v>
+        <v>10305</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D42" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>10205</v>
+        <v>10310</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>10210</v>
+        <v>10315</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D44" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>10215</v>
+        <v>10320</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D45" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>10220</v>
+        <v>10325</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="D46" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>10225</v>
+        <v>10330</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D47" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>10230</v>
+        <v>10335</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="D48" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>10235</v>
+        <v>10340</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="D49" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>10240</v>
+        <v>10345</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="D50" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>10245</v>
+        <v>10350</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="D51" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>10250</v>
+        <v>10355</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="D52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>10255</v>
+        <v>10360</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>10260</v>
+        <v>10365</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>10265</v>
+        <v>10370</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D55" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>10270</v>
+        <v>10375</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>10275</v>
+        <v>10380</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="D57" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>10280</v>
+        <v>10385</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D58" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>10285</v>
+        <v>10390</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="D59" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>10290</v>
+        <v>10395</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D60" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>10295</v>
+        <v>10400</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D61" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>10300</v>
+        <v>10405</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="D62" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>10305</v>
+        <v>10410</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D63" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>10310</v>
+        <v>10415</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="D64" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>10315</v>
+        <v>10420</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D65" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>10320</v>
+        <v>10425</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>10325</v>
+        <v>10430</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>10330</v>
+        <v>10435</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D68" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>10335</v>
+        <v>10440</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D69" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>10340</v>
+        <v>10445</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="D70" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>10345</v>
+        <v>10450</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="D71" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>10350</v>
+        <v>10455</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D72" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>10355</v>
-      </c>
-      <c r="B73" s="2"/>
+        <v>10460</v>
+      </c>
+      <c r="B73" s="2">
+        <v>12</v>
+      </c>
       <c r="C73" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D73" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>10360</v>
-      </c>
-      <c r="B74" s="2"/>
+        <v>10465</v>
+      </c>
+      <c r="B74" s="2">
+        <v>20</v>
+      </c>
       <c r="C74" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D74" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>10365</v>
-      </c>
-      <c r="B75" s="2"/>
+        <v>10470</v>
+      </c>
+      <c r="B75" s="2">
+        <v>6</v>
+      </c>
       <c r="C75" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D75" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>10370</v>
-      </c>
-      <c r="B76" s="2"/>
+        <v>10475</v>
+      </c>
+      <c r="B76" s="2">
+        <v>11</v>
+      </c>
       <c r="C76" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D76" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>10375</v>
-      </c>
-      <c r="B77" s="2"/>
+        <v>10480</v>
+      </c>
+      <c r="B77" s="2">
+        <v>9</v>
+      </c>
       <c r="C77" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D77" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>10380</v>
-      </c>
-      <c r="B78" s="2"/>
+        <v>10485</v>
+      </c>
+      <c r="B78" s="2">
+        <v>17</v>
+      </c>
       <c r="C78" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D78" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>10385</v>
-      </c>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D79" t="s">
-        <v>38</v>
+        <v>10490</v>
+      </c>
+      <c r="B79" s="2">
+        <v>16</v>
+      </c>
+      <c r="C79" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>10390</v>
-      </c>
-      <c r="B80" s="2"/>
+        <v>10495</v>
+      </c>
+      <c r="B80" s="2">
+        <v>3</v>
+      </c>
       <c r="C80" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D80" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>10500</v>
+      </c>
+      <c r="B81" s="2">
+        <v>13</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>10505</v>
+      </c>
+      <c r="B82" s="2">
+        <v>19</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>10510</v>
+      </c>
+      <c r="B83" s="2">
+        <v>4</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>10515</v>
+      </c>
+      <c r="B84" s="2">
+        <v>18</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>10520</v>
+      </c>
+      <c r="B85" s="2">
+        <v>1</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>10525</v>
+      </c>
+      <c r="B86" s="2">
+        <v>15</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>10530</v>
+      </c>
+      <c r="B87" s="2">
+        <v>7</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>10535</v>
+      </c>
+      <c r="B88" s="2">
+        <v>10</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
-        <v>10395</v>
-      </c>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D81" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>10540</v>
+      </c>
+      <c r="B89" s="2">
+        <v>14</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
-        <v>10400</v>
-      </c>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D82" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>10545</v>
+      </c>
+      <c r="B90" s="2">
+        <v>2</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
-        <v>10405</v>
-      </c>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D83" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
-        <v>10410</v>
-      </c>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D84" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>10550</v>
+      </c>
+      <c r="B91" s="2">
+        <v>8</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
-        <v>10415</v>
-      </c>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D85" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
-        <v>10420</v>
-      </c>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D86" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
-        <v>10425</v>
-      </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D87" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
-        <v>10430</v>
-      </c>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D88" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>10555</v>
+      </c>
+      <c r="B92" s="2">
+        <v>5</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
-        <v>10435</v>
-      </c>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D89" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
-        <v>10440</v>
-      </c>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D90" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
-        <v>10445</v>
-      </c>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D91" t="s">
-        <v>82</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D91">
-    <sortCondition ref="D22:D91"/>
-    <sortCondition ref="C22:C91"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D93">
+    <sortCondition ref="D1:D93"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UPDATED: excel & json
</commit_message>
<xml_diff>
--- a/data/common/excel/public_categories_odoo.xlsx
+++ b/data/common/excel/public_categories_odoo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OPT Design\PycharmProjects\optima-scrapper\data\common\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8860971-77A5-46D9-AA16-E00B53CEDF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79943AE5-B894-403E-9C8C-417B5C1F2F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,1079 +662,1081 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>10105</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>10520</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>10110</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>10545</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>10115</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>10495</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>10120</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>10510</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>10125</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>10555</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>10130</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>10470</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>10135</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>10530</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>10140</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>10550</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>10145</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>10480</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>10150</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>10535</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>10155</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>10475</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>10160</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>10460</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>10165</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>10500</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>10170</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>10540</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>10175</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>10525</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
       <c r="C16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>10180</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" t="s">
+        <v>10490</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>10185</v>
-      </c>
-      <c r="B18" s="2"/>
+        <v>10485</v>
+      </c>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
       <c r="C18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>10190</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>10515</v>
+      </c>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
       <c r="C19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>10195</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>10505</v>
+      </c>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
       <c r="C20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>10200</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>10465</v>
+      </c>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>10205</v>
+        <v>10105</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>10210</v>
+        <v>10110</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>10215</v>
+        <v>10115</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>10220</v>
+        <v>10120</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>10225</v>
+        <v>10125</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>10230</v>
+        <v>10130</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>10235</v>
+        <v>10135</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>10240</v>
+        <v>10140</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>10245</v>
+        <v>10145</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>10250</v>
+        <v>10150</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>10255</v>
+        <v>10155</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>10260</v>
+        <v>10160</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>10265</v>
+        <v>10165</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>10270</v>
+        <v>10170</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>10275</v>
+        <v>10175</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>10280</v>
+        <v>10180</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>10285</v>
+        <v>10185</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>10290</v>
+        <v>10190</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>10295</v>
+        <v>10195</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>10300</v>
+        <v>10200</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>10305</v>
+        <v>10205</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>10310</v>
+        <v>10210</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>10315</v>
+        <v>10215</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D44" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>10320</v>
+        <v>10220</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D45" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>10325</v>
+        <v>10225</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="D46" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>10330</v>
+        <v>10230</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D47" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>10335</v>
+        <v>10235</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>10340</v>
+        <v>10240</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>10345</v>
+        <v>10245</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>10350</v>
+        <v>10250</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>10355</v>
+        <v>10255</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>10360</v>
+        <v>10260</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>10365</v>
+        <v>10265</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>10370</v>
+        <v>10270</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>10375</v>
+        <v>10275</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D56" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>10380</v>
+        <v>10280</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>10385</v>
+        <v>10285</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D58" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>10390</v>
+        <v>10290</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="D59" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>10395</v>
+        <v>10295</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D60" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>10400</v>
+        <v>10300</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D61" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>10405</v>
+        <v>10305</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="D62" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>10410</v>
+        <v>10310</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="D63" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>10415</v>
+        <v>10315</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D64" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>10420</v>
+        <v>10320</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="D65" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>10425</v>
+        <v>10325</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D66" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>10430</v>
+        <v>10330</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="D67" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>10435</v>
+        <v>10335</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="D68" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>10440</v>
+        <v>10340</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="D69" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>10445</v>
+        <v>10345</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="D70" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>10450</v>
+        <v>10350</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="D71" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>10455</v>
+        <v>10355</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="D72" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>10460</v>
-      </c>
-      <c r="B73" s="2">
-        <v>12</v>
-      </c>
+        <v>10360</v>
+      </c>
+      <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>10465</v>
-      </c>
-      <c r="B74" s="2">
-        <v>20</v>
-      </c>
+        <v>10365</v>
+      </c>
+      <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>65</v>
+        <v>17</v>
+      </c>
+      <c r="D74" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>10470</v>
-      </c>
-      <c r="B75" s="2">
-        <v>6</v>
-      </c>
+        <v>10370</v>
+      </c>
+      <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>6</v>
+        <v>33</v>
+      </c>
+      <c r="D75" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>10475</v>
-      </c>
-      <c r="B76" s="2">
-        <v>11</v>
-      </c>
+        <v>10375</v>
+      </c>
+      <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
+      </c>
+      <c r="D76" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>10480</v>
-      </c>
-      <c r="B77" s="2">
-        <v>9</v>
-      </c>
+        <v>10380</v>
+      </c>
+      <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>59</v>
+        <v>78</v>
+      </c>
+      <c r="D77" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>10485</v>
-      </c>
-      <c r="B78" s="2">
-        <v>17</v>
-      </c>
+        <v>10385</v>
+      </c>
+      <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>63</v>
+        <v>40</v>
+      </c>
+      <c r="D78" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>10490</v>
-      </c>
-      <c r="B79" s="2">
-        <v>16</v>
-      </c>
-      <c r="C79" t="s">
-        <v>54</v>
+        <v>10390</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D79" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>10495</v>
-      </c>
-      <c r="B80" s="2">
-        <v>3</v>
-      </c>
+        <v>10395</v>
+      </c>
+      <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="D80" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>10500</v>
-      </c>
-      <c r="B81" s="2">
-        <v>13</v>
-      </c>
+        <v>10400</v>
+      </c>
+      <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="D81" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>10505</v>
-      </c>
-      <c r="B82" s="2">
-        <v>19</v>
-      </c>
+        <v>10405</v>
+      </c>
+      <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="D82" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>10510</v>
-      </c>
-      <c r="B83" s="2">
-        <v>4</v>
-      </c>
+        <v>10410</v>
+      </c>
+      <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>10515</v>
-      </c>
-      <c r="B84" s="2">
-        <v>18</v>
-      </c>
+        <v>10415</v>
+      </c>
+      <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="D84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>10520</v>
-      </c>
-      <c r="B85" s="2">
+        <v>10420</v>
+      </c>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D85" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>10425</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
-        <v>10525</v>
-      </c>
-      <c r="B86" s="2">
-        <v>15</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>10530</v>
-      </c>
-      <c r="B87" s="2">
-        <v>7</v>
-      </c>
+        <v>10430</v>
+      </c>
+      <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D87" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>10535</v>
-      </c>
-      <c r="B88" s="2">
-        <v>10</v>
-      </c>
+        <v>10435</v>
+      </c>
+      <c r="B88" s="2"/>
       <c r="C88" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D88" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>10540</v>
-      </c>
-      <c r="B89" s="2">
-        <v>14</v>
-      </c>
+        <v>10440</v>
+      </c>
+      <c r="B89" s="2"/>
       <c r="C89" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="D89" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>10545</v>
-      </c>
-      <c r="B90" s="2">
-        <v>2</v>
-      </c>
+        <v>10445</v>
+      </c>
+      <c r="B90" s="2"/>
       <c r="C90" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="D90" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>10550</v>
-      </c>
-      <c r="B91" s="2">
-        <v>8</v>
-      </c>
+        <v>10450</v>
+      </c>
+      <c r="B91" s="2"/>
       <c r="C91" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D91" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>10555</v>
-      </c>
-      <c r="B92" s="2">
-        <v>5</v>
-      </c>
+        <v>10455</v>
+      </c>
+      <c r="B92" s="2"/>
       <c r="C92" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D92" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D93">
-    <sortCondition ref="D1:D93"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D94">
+    <sortCondition ref="B2:B94"/>
+    <sortCondition ref="D2:D94"/>
+    <sortCondition ref="C2:C94"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>